<commit_message>
color tracking gold plating
</commit_message>
<xml_diff>
--- a/docs/panTiltCalibration.xlsx
+++ b/docs/panTiltCalibration.xlsx
@@ -4,18 +4,19 @@
   <fileVersion appName="xl" lastEdited="6" lowestEdited="6" rupBuild="14420"/>
   <workbookPr filterPrivacy="1" defaultThemeVersion="124226"/>
   <bookViews>
-    <workbookView xWindow="240" yWindow="105" windowWidth="14805" windowHeight="8010" activeTab="1"/>
+    <workbookView xWindow="240" yWindow="105" windowWidth="14805" windowHeight="8010"/>
   </bookViews>
   <sheets>
-    <sheet name="Pan Regrssion" sheetId="2" r:id="rId1"/>
-    <sheet name="Sheet1" sheetId="1" r:id="rId2"/>
+    <sheet name="Observations" sheetId="1" r:id="rId1"/>
+    <sheet name="Pan Regression" sheetId="2" r:id="rId2"/>
+    <sheet name="Tilt Regression" sheetId="4" r:id="rId3"/>
   </sheets>
   <calcPr calcId="152511"/>
 </workbook>
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="37" uniqueCount="35">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="64" uniqueCount="38">
   <si>
     <t>From</t>
   </si>
@@ -122,12 +123,21 @@
   <si>
     <t>X Variable 1</t>
   </si>
+  <si>
+    <t>Linear Regression Test</t>
+  </si>
+  <si>
+    <t>Lower 98.0%</t>
+  </si>
+  <si>
+    <t>Upper 98.0%</t>
+  </si>
 </sst>
 </file>
 
 <file path=xl/styles.xml><?xml version="1.0" encoding="utf-8"?>
 <styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
-  <fonts count="4" x14ac:knownFonts="1">
+  <fonts count="5" x14ac:knownFonts="1">
     <font>
       <sz val="11"/>
       <color theme="1"/>
@@ -159,16 +169,29 @@
       <family val="2"/>
       <scheme val="minor"/>
     </font>
+    <font>
+      <b/>
+      <sz val="11"/>
+      <color rgb="FFFA7D00"/>
+      <name val="Calibri"/>
+      <family val="2"/>
+      <scheme val="minor"/>
+    </font>
   </fonts>
-  <fills count="2">
+  <fills count="3">
     <fill>
       <patternFill patternType="none"/>
     </fill>
     <fill>
       <patternFill patternType="gray125"/>
     </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor rgb="FFF2F2F2"/>
+      </patternFill>
+    </fill>
   </fills>
-  <borders count="5">
+  <borders count="6">
     <border>
       <left/>
       <right/>
@@ -214,13 +237,29 @@
       </bottom>
       <diagonal/>
     </border>
+    <border>
+      <left style="thin">
+        <color rgb="FF7F7F7F"/>
+      </left>
+      <right style="thin">
+        <color rgb="FF7F7F7F"/>
+      </right>
+      <top style="thin">
+        <color rgb="FF7F7F7F"/>
+      </top>
+      <bottom style="thin">
+        <color rgb="FF7F7F7F"/>
+      </bottom>
+      <diagonal/>
+    </border>
   </borders>
-  <cellStyleXfs count="3">
+  <cellStyleXfs count="4">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
     <xf numFmtId="0" fontId="1" fillId="0" borderId="1" applyNumberFormat="0" applyFill="0" applyAlignment="0" applyProtection="0"/>
     <xf numFmtId="0" fontId="2" fillId="0" borderId="2" applyNumberFormat="0" applyFill="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="4" fillId="2" borderId="5" applyNumberFormat="0" applyAlignment="0" applyProtection="0"/>
   </cellStyleXfs>
-  <cellXfs count="10">
+  <cellXfs count="11">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="0" fontId="1" fillId="0" borderId="1" xfId="1"/>
     <xf numFmtId="0" fontId="2" fillId="0" borderId="2" xfId="2"/>
@@ -237,8 +276,10 @@
     <xf numFmtId="0" fontId="3" fillId="0" borderId="4" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="centerContinuous"/>
     </xf>
+    <xf numFmtId="0" fontId="4" fillId="2" borderId="5" xfId="3"/>
   </cellXfs>
-  <cellStyles count="3">
+  <cellStyles count="4">
+    <cellStyle name="Calculation" xfId="3" builtinId="22"/>
     <cellStyle name="Heading 2" xfId="1" builtinId="17"/>
     <cellStyle name="Heading 3" xfId="2" builtinId="18"/>
     <cellStyle name="Normal" xfId="0" builtinId="0"/>
@@ -295,7 +336,7 @@
             </a:r>
             <a:r>
               <a:rPr lang="en-AU" baseline="0"/>
-              <a:t> Movement</a:t>
+              <a:t> Axis</a:t>
             </a:r>
           </a:p>
         </c:rich>
@@ -344,16 +385,14 @@
         </c:manualLayout>
       </c:layout>
       <c:scatterChart>
-        <c:scatterStyle val="smoothMarker"/>
+        <c:scatterStyle val="lineMarker"/>
         <c:varyColors val="0"/>
         <c:ser>
           <c:idx val="0"/>
           <c:order val="0"/>
           <c:spPr>
-            <a:ln w="19050" cap="rnd">
-              <a:solidFill>
-                <a:schemeClr val="accent1"/>
-              </a:solidFill>
+            <a:ln w="25400" cap="rnd">
+              <a:noFill/>
               <a:round/>
             </a:ln>
             <a:effectLst/>
@@ -432,7 +471,12 @@
             <c:dispRSqr val="1"/>
             <c:dispEq val="1"/>
             <c:trendlineLbl>
-              <c:layout/>
+              <c:layout>
+                <c:manualLayout>
+                  <c:x val="2.8494709054739916E-3"/>
+                  <c:y val="-9.9151468513765002E-3"/>
+                </c:manualLayout>
+              </c:layout>
               <c:numFmt formatCode="General" sourceLinked="0"/>
               <c:spPr>
                 <a:noFill/>
@@ -465,7 +509,7 @@
           </c:trendline>
           <c:xVal>
             <c:numRef>
-              <c:f>Sheet1!$C$5:$C$15</c:f>
+              <c:f>Observations!$C$5:$C$15</c:f>
               <c:numCache>
                 <c:formatCode>#,##0</c:formatCode>
                 <c:ptCount val="11"/>
@@ -507,7 +551,7 @@
           </c:xVal>
           <c:yVal>
             <c:numRef>
-              <c:f>Sheet1!$E$5:$E$15</c:f>
+              <c:f>Observations!$E$5:$E$15</c:f>
               <c:numCache>
                 <c:formatCode>0.00</c:formatCode>
                 <c:ptCount val="11"/>
@@ -547,7 +591,7 @@
               </c:numCache>
             </c:numRef>
           </c:yVal>
-          <c:smooth val="1"/>
+          <c:smooth val="0"/>
         </c:ser>
         <c:dLbls>
           <c:showLegendKey val="0"/>
@@ -557,11 +601,11 @@
           <c:showPercent val="0"/>
           <c:showBubbleSize val="0"/>
         </c:dLbls>
-        <c:axId val="442947800"/>
-        <c:axId val="442957992"/>
+        <c:axId val="299493920"/>
+        <c:axId val="299504504"/>
       </c:scatterChart>
       <c:valAx>
-        <c:axId val="442947800"/>
+        <c:axId val="299493920"/>
         <c:scaling>
           <c:orientation val="minMax"/>
         </c:scaling>
@@ -581,6 +625,62 @@
             <a:effectLst/>
           </c:spPr>
         </c:majorGridlines>
+        <c:title>
+          <c:tx>
+            <c:rich>
+              <a:bodyPr rot="0" spcFirstLastPara="1" vertOverflow="ellipsis" vert="horz" wrap="square" anchor="ctr" anchorCtr="1"/>
+              <a:lstStyle/>
+              <a:p>
+                <a:pPr>
+                  <a:defRPr sz="1000" b="0" i="0" u="none" strike="noStrike" kern="1200" baseline="0">
+                    <a:solidFill>
+                      <a:schemeClr val="tx1">
+                        <a:lumMod val="65000"/>
+                        <a:lumOff val="35000"/>
+                      </a:schemeClr>
+                    </a:solidFill>
+                    <a:latin typeface="+mn-lt"/>
+                    <a:ea typeface="+mn-ea"/>
+                    <a:cs typeface="+mn-cs"/>
+                  </a:defRPr>
+                </a:pPr>
+                <a:r>
+                  <a:rPr lang="en-AU"/>
+                  <a:t>Pixels from Center</a:t>
+                </a:r>
+              </a:p>
+            </c:rich>
+          </c:tx>
+          <c:layout/>
+          <c:overlay val="0"/>
+          <c:spPr>
+            <a:noFill/>
+            <a:ln>
+              <a:noFill/>
+            </a:ln>
+            <a:effectLst/>
+          </c:spPr>
+          <c:txPr>
+            <a:bodyPr rot="0" spcFirstLastPara="1" vertOverflow="ellipsis" vert="horz" wrap="square" anchor="ctr" anchorCtr="1"/>
+            <a:lstStyle/>
+            <a:p>
+              <a:pPr>
+                <a:defRPr sz="1000" b="0" i="0" u="none" strike="noStrike" kern="1200" baseline="0">
+                  <a:solidFill>
+                    <a:schemeClr val="tx1">
+                      <a:lumMod val="65000"/>
+                      <a:lumOff val="35000"/>
+                    </a:schemeClr>
+                  </a:solidFill>
+                  <a:latin typeface="+mn-lt"/>
+                  <a:ea typeface="+mn-ea"/>
+                  <a:cs typeface="+mn-cs"/>
+                </a:defRPr>
+              </a:pPr>
+              <a:endParaRPr lang="en-US"/>
+            </a:p>
+          </c:txPr>
+        </c:title>
         <c:numFmt formatCode="#,##0" sourceLinked="1"/>
         <c:majorTickMark val="none"/>
         <c:minorTickMark val="none"/>
@@ -618,12 +718,12 @@
             <a:endParaRPr lang="en-US"/>
           </a:p>
         </c:txPr>
-        <c:crossAx val="442957992"/>
+        <c:crossAx val="299504504"/>
         <c:crosses val="autoZero"/>
         <c:crossBetween val="midCat"/>
       </c:valAx>
       <c:valAx>
-        <c:axId val="442957992"/>
+        <c:axId val="299504504"/>
         <c:scaling>
           <c:orientation val="minMax"/>
         </c:scaling>
@@ -643,6 +743,74 @@
             <a:effectLst/>
           </c:spPr>
         </c:majorGridlines>
+        <c:title>
+          <c:tx>
+            <c:rich>
+              <a:bodyPr rot="-5400000" spcFirstLastPara="1" vertOverflow="ellipsis" vert="horz" wrap="square" anchor="ctr" anchorCtr="1"/>
+              <a:lstStyle/>
+              <a:p>
+                <a:pPr>
+                  <a:defRPr sz="1000" b="0" i="0" u="none" strike="noStrike" kern="1200" baseline="0">
+                    <a:solidFill>
+                      <a:schemeClr val="tx1">
+                        <a:lumMod val="65000"/>
+                        <a:lumOff val="35000"/>
+                      </a:schemeClr>
+                    </a:solidFill>
+                    <a:latin typeface="+mn-lt"/>
+                    <a:ea typeface="+mn-ea"/>
+                    <a:cs typeface="+mn-cs"/>
+                  </a:defRPr>
+                </a:pPr>
+                <a:r>
+                  <a:rPr lang="en-AU"/>
+                  <a:t>Servo Perentage required</a:t>
+                </a:r>
+                <a:r>
+                  <a:rPr lang="en-AU" baseline="0"/>
+                  <a:t> to Center</a:t>
+                </a:r>
+                <a:endParaRPr lang="en-AU"/>
+              </a:p>
+            </c:rich>
+          </c:tx>
+          <c:layout>
+            <c:manualLayout>
+              <c:xMode val="edge"/>
+              <c:yMode val="edge"/>
+              <c:x val="9.8643793445127737E-3"/>
+              <c:y val="0.3281005168689558"/>
+            </c:manualLayout>
+          </c:layout>
+          <c:overlay val="0"/>
+          <c:spPr>
+            <a:noFill/>
+            <a:ln>
+              <a:noFill/>
+            </a:ln>
+            <a:effectLst/>
+          </c:spPr>
+          <c:txPr>
+            <a:bodyPr rot="-5400000" spcFirstLastPara="1" vertOverflow="ellipsis" vert="horz" wrap="square" anchor="ctr" anchorCtr="1"/>
+            <a:lstStyle/>
+            <a:p>
+              <a:pPr>
+                <a:defRPr sz="1000" b="0" i="0" u="none" strike="noStrike" kern="1200" baseline="0">
+                  <a:solidFill>
+                    <a:schemeClr val="tx1">
+                      <a:lumMod val="65000"/>
+                      <a:lumOff val="35000"/>
+                    </a:schemeClr>
+                  </a:solidFill>
+                  <a:latin typeface="+mn-lt"/>
+                  <a:ea typeface="+mn-ea"/>
+                  <a:cs typeface="+mn-cs"/>
+                </a:defRPr>
+              </a:pPr>
+              <a:endParaRPr lang="en-US"/>
+            </a:p>
+          </c:txPr>
+        </c:title>
         <c:numFmt formatCode="0.00" sourceLinked="1"/>
         <c:majorTickMark val="none"/>
         <c:minorTickMark val="none"/>
@@ -680,7 +848,7 @@
             <a:endParaRPr lang="en-US"/>
           </a:p>
         </c:txPr>
-        <c:crossAx val="442947800"/>
+        <c:crossAx val="299493920"/>
         <c:crosses val="autoZero"/>
         <c:crossBetween val="midCat"/>
       </c:valAx>
@@ -764,7 +932,7 @@
             </a:pPr>
             <a:r>
               <a:rPr lang="en-AU"/>
-              <a:t>Tilt Movement</a:t>
+              <a:t>Tilt Axis</a:t>
             </a:r>
           </a:p>
         </c:rich>
@@ -803,16 +971,14 @@
     <c:plotArea>
       <c:layout/>
       <c:scatterChart>
-        <c:scatterStyle val="smoothMarker"/>
+        <c:scatterStyle val="lineMarker"/>
         <c:varyColors val="0"/>
         <c:ser>
           <c:idx val="0"/>
           <c:order val="0"/>
           <c:spPr>
-            <a:ln w="19050" cap="rnd">
-              <a:solidFill>
-                <a:schemeClr val="accent1"/>
-              </a:solidFill>
+            <a:ln w="25400" cap="rnd">
+              <a:noFill/>
               <a:round/>
             </a:ln>
             <a:effectLst/>
@@ -884,7 +1050,7 @@
           </c:trendline>
           <c:xVal>
             <c:numRef>
-              <c:f>Sheet1!$C$18:$C$28</c:f>
+              <c:f>Observations!$C$18:$C$28</c:f>
               <c:numCache>
                 <c:formatCode>#,##0</c:formatCode>
                 <c:ptCount val="11"/>
@@ -926,7 +1092,7 @@
           </c:xVal>
           <c:yVal>
             <c:numRef>
-              <c:f>Sheet1!$E$18:$E$28</c:f>
+              <c:f>Observations!$E$18:$E$28</c:f>
               <c:numCache>
                 <c:formatCode>0.00</c:formatCode>
                 <c:ptCount val="11"/>
@@ -966,7 +1132,7 @@
               </c:numCache>
             </c:numRef>
           </c:yVal>
-          <c:smooth val="1"/>
+          <c:smooth val="0"/>
         </c:ser>
         <c:dLbls>
           <c:showLegendKey val="0"/>
@@ -976,11 +1142,11 @@
           <c:showPercent val="0"/>
           <c:showBubbleSize val="0"/>
         </c:dLbls>
-        <c:axId val="442946624"/>
-        <c:axId val="442954072"/>
+        <c:axId val="299498624"/>
+        <c:axId val="299495880"/>
       </c:scatterChart>
       <c:valAx>
-        <c:axId val="442946624"/>
+        <c:axId val="299498624"/>
         <c:scaling>
           <c:orientation val="minMax"/>
         </c:scaling>
@@ -1000,6 +1166,62 @@
             <a:effectLst/>
           </c:spPr>
         </c:majorGridlines>
+        <c:title>
+          <c:tx>
+            <c:rich>
+              <a:bodyPr rot="0" spcFirstLastPara="1" vertOverflow="ellipsis" vert="horz" wrap="square" anchor="ctr" anchorCtr="1"/>
+              <a:lstStyle/>
+              <a:p>
+                <a:pPr>
+                  <a:defRPr sz="1000" b="0" i="0" u="none" strike="noStrike" kern="1200" baseline="0">
+                    <a:solidFill>
+                      <a:schemeClr val="tx1">
+                        <a:lumMod val="65000"/>
+                        <a:lumOff val="35000"/>
+                      </a:schemeClr>
+                    </a:solidFill>
+                    <a:latin typeface="+mn-lt"/>
+                    <a:ea typeface="+mn-ea"/>
+                    <a:cs typeface="+mn-cs"/>
+                  </a:defRPr>
+                </a:pPr>
+                <a:r>
+                  <a:rPr lang="en-AU"/>
+                  <a:t>Pixels from Center</a:t>
+                </a:r>
+              </a:p>
+            </c:rich>
+          </c:tx>
+          <c:layout/>
+          <c:overlay val="0"/>
+          <c:spPr>
+            <a:noFill/>
+            <a:ln>
+              <a:noFill/>
+            </a:ln>
+            <a:effectLst/>
+          </c:spPr>
+          <c:txPr>
+            <a:bodyPr rot="0" spcFirstLastPara="1" vertOverflow="ellipsis" vert="horz" wrap="square" anchor="ctr" anchorCtr="1"/>
+            <a:lstStyle/>
+            <a:p>
+              <a:pPr>
+                <a:defRPr sz="1000" b="0" i="0" u="none" strike="noStrike" kern="1200" baseline="0">
+                  <a:solidFill>
+                    <a:schemeClr val="tx1">
+                      <a:lumMod val="65000"/>
+                      <a:lumOff val="35000"/>
+                    </a:schemeClr>
+                  </a:solidFill>
+                  <a:latin typeface="+mn-lt"/>
+                  <a:ea typeface="+mn-ea"/>
+                  <a:cs typeface="+mn-cs"/>
+                </a:defRPr>
+              </a:pPr>
+              <a:endParaRPr lang="en-US"/>
+            </a:p>
+          </c:txPr>
+        </c:title>
         <c:numFmt formatCode="#,##0" sourceLinked="1"/>
         <c:majorTickMark val="none"/>
         <c:minorTickMark val="none"/>
@@ -1037,12 +1259,12 @@
             <a:endParaRPr lang="en-US"/>
           </a:p>
         </c:txPr>
-        <c:crossAx val="442954072"/>
+        <c:crossAx val="299495880"/>
         <c:crosses val="autoZero"/>
         <c:crossBetween val="midCat"/>
       </c:valAx>
       <c:valAx>
-        <c:axId val="442954072"/>
+        <c:axId val="299495880"/>
         <c:scaling>
           <c:orientation val="minMax"/>
         </c:scaling>
@@ -1062,6 +1284,69 @@
             <a:effectLst/>
           </c:spPr>
         </c:majorGridlines>
+        <c:title>
+          <c:tx>
+            <c:rich>
+              <a:bodyPr rot="-5400000" spcFirstLastPara="1" vertOverflow="ellipsis" vert="horz" wrap="square" anchor="ctr" anchorCtr="1"/>
+              <a:lstStyle/>
+              <a:p>
+                <a:pPr>
+                  <a:defRPr sz="1000" b="0" i="0" u="none" strike="noStrike" kern="1200" baseline="0">
+                    <a:solidFill>
+                      <a:schemeClr val="tx1">
+                        <a:lumMod val="65000"/>
+                        <a:lumOff val="35000"/>
+                      </a:schemeClr>
+                    </a:solidFill>
+                    <a:latin typeface="+mn-lt"/>
+                    <a:ea typeface="+mn-ea"/>
+                    <a:cs typeface="+mn-cs"/>
+                  </a:defRPr>
+                </a:pPr>
+                <a:r>
+                  <a:rPr lang="en-AU"/>
+                  <a:t>Servo Percentage requried to Center</a:t>
+                </a:r>
+              </a:p>
+            </c:rich>
+          </c:tx>
+          <c:layout>
+            <c:manualLayout>
+              <c:xMode val="edge"/>
+              <c:yMode val="edge"/>
+              <c:x val="1.2544802867383513E-2"/>
+              <c:y val="0.17443853325028202"/>
+            </c:manualLayout>
+          </c:layout>
+          <c:overlay val="0"/>
+          <c:spPr>
+            <a:noFill/>
+            <a:ln>
+              <a:noFill/>
+            </a:ln>
+            <a:effectLst/>
+          </c:spPr>
+          <c:txPr>
+            <a:bodyPr rot="-5400000" spcFirstLastPara="1" vertOverflow="ellipsis" vert="horz" wrap="square" anchor="ctr" anchorCtr="1"/>
+            <a:lstStyle/>
+            <a:p>
+              <a:pPr>
+                <a:defRPr sz="1000" b="0" i="0" u="none" strike="noStrike" kern="1200" baseline="0">
+                  <a:solidFill>
+                    <a:schemeClr val="tx1">
+                      <a:lumMod val="65000"/>
+                      <a:lumOff val="35000"/>
+                    </a:schemeClr>
+                  </a:solidFill>
+                  <a:latin typeface="+mn-lt"/>
+                  <a:ea typeface="+mn-ea"/>
+                  <a:cs typeface="+mn-cs"/>
+                </a:defRPr>
+              </a:pPr>
+              <a:endParaRPr lang="en-US"/>
+            </a:p>
+          </c:txPr>
+        </c:title>
         <c:numFmt formatCode="0.00" sourceLinked="1"/>
         <c:majorTickMark val="none"/>
         <c:minorTickMark val="none"/>
@@ -1099,7 +1384,7 @@
             <a:endParaRPr lang="en-US"/>
           </a:p>
         </c:txPr>
-        <c:crossAx val="442946624"/>
+        <c:crossAx val="299498624"/>
         <c:crosses val="autoZero"/>
         <c:crossBetween val="midCat"/>
       </c:valAx>
@@ -2264,16 +2549,16 @@
 <xdr:wsDr xmlns:xdr="http://schemas.openxmlformats.org/drawingml/2006/spreadsheetDrawing" xmlns:a="http://schemas.openxmlformats.org/drawingml/2006/main">
   <xdr:twoCellAnchor>
     <xdr:from>
-      <xdr:col>5</xdr:col>
-      <xdr:colOff>304800</xdr:colOff>
-      <xdr:row>4</xdr:row>
-      <xdr:rowOff>14287</xdr:rowOff>
+      <xdr:col>6</xdr:col>
+      <xdr:colOff>314325</xdr:colOff>
+      <xdr:row>2</xdr:row>
+      <xdr:rowOff>128587</xdr:rowOff>
     </xdr:from>
     <xdr:to>
-      <xdr:col>16</xdr:col>
-      <xdr:colOff>209550</xdr:colOff>
-      <xdr:row>26</xdr:row>
-      <xdr:rowOff>142875</xdr:rowOff>
+      <xdr:col>17</xdr:col>
+      <xdr:colOff>219075</xdr:colOff>
+      <xdr:row>25</xdr:row>
+      <xdr:rowOff>28575</xdr:rowOff>
     </xdr:to>
     <xdr:graphicFrame macro="">
       <xdr:nvGraphicFramePr>
@@ -2294,16 +2579,16 @@
   </xdr:twoCellAnchor>
   <xdr:twoCellAnchor>
     <xdr:from>
-      <xdr:col>4</xdr:col>
-      <xdr:colOff>914400</xdr:colOff>
-      <xdr:row>27</xdr:row>
-      <xdr:rowOff>71437</xdr:rowOff>
+      <xdr:col>6</xdr:col>
+      <xdr:colOff>266700</xdr:colOff>
+      <xdr:row>25</xdr:row>
+      <xdr:rowOff>147637</xdr:rowOff>
     </xdr:from>
     <xdr:to>
-      <xdr:col>16</xdr:col>
-      <xdr:colOff>257175</xdr:colOff>
-      <xdr:row>41</xdr:row>
-      <xdr:rowOff>104775</xdr:rowOff>
+      <xdr:col>18</xdr:col>
+      <xdr:colOff>38100</xdr:colOff>
+      <xdr:row>39</xdr:row>
+      <xdr:rowOff>180975</xdr:rowOff>
     </xdr:to>
     <xdr:graphicFrame macro="">
       <xdr:nvGraphicFramePr>
@@ -2612,10 +2897,592 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
+  <dimension ref="A1:F28"/>
+  <sheetViews>
+    <sheetView tabSelected="1" workbookViewId="0">
+      <selection activeCell="C28" sqref="C28"/>
+    </sheetView>
+  </sheetViews>
+  <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
+  <cols>
+    <col min="1" max="1" width="15.28515625" customWidth="1"/>
+    <col min="2" max="4" width="13.7109375" customWidth="1"/>
+    <col min="5" max="5" width="19.42578125" customWidth="1"/>
+  </cols>
+  <sheetData>
+    <row r="1" spans="1:6" s="2" customFormat="1" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
+      <c r="A1" s="2" t="s">
+        <v>5</v>
+      </c>
+    </row>
+    <row r="2" spans="1:6" s="2" customFormat="1" ht="30.75" thickBot="1" x14ac:dyDescent="0.3">
+      <c r="A2" s="2" t="s">
+        <v>0</v>
+      </c>
+      <c r="B2" s="2" t="s">
+        <v>1</v>
+      </c>
+      <c r="D2" s="2" t="s">
+        <v>2</v>
+      </c>
+      <c r="E2" s="4" t="s">
+        <v>6</v>
+      </c>
+    </row>
+    <row r="3" spans="1:6" x14ac:dyDescent="0.25">
+      <c r="B3" t="s">
+        <v>4</v>
+      </c>
+    </row>
+    <row r="4" spans="1:6" ht="18" thickBot="1" x14ac:dyDescent="0.35">
+      <c r="A4" s="1" t="s">
+        <v>2</v>
+      </c>
+      <c r="C4" t="s">
+        <v>8</v>
+      </c>
+      <c r="D4" t="s">
+        <v>7</v>
+      </c>
+      <c r="E4" t="s">
+        <v>9</v>
+      </c>
+      <c r="F4" s="10" t="s">
+        <v>35</v>
+      </c>
+    </row>
+    <row r="5" spans="1:6" ht="15.75" thickTop="1" x14ac:dyDescent="0.25">
+      <c r="A5">
+        <v>5</v>
+      </c>
+      <c r="B5" s="3">
+        <v>160</v>
+      </c>
+      <c r="C5" s="3">
+        <f>B5-A5</f>
+        <v>155</v>
+      </c>
+      <c r="D5" s="5">
+        <v>64</v>
+      </c>
+      <c r="E5" s="5">
+        <f>D5-50</f>
+        <v>14</v>
+      </c>
+      <c r="F5" s="10">
+        <f>C5*0.0933</f>
+        <v>14.461499999999999</v>
+      </c>
+    </row>
+    <row r="6" spans="1:6" x14ac:dyDescent="0.25">
+      <c r="A6">
+        <v>32</v>
+      </c>
+      <c r="B6" s="3">
+        <v>160</v>
+      </c>
+      <c r="C6" s="3">
+        <f t="shared" ref="C6:C28" si="0">B6-A6</f>
+        <v>128</v>
+      </c>
+      <c r="D6" s="5">
+        <v>62.3</v>
+      </c>
+      <c r="E6" s="5">
+        <f t="shared" ref="E6:E28" si="1">D6-50</f>
+        <v>12.299999999999997</v>
+      </c>
+      <c r="F6" s="10">
+        <f t="shared" ref="F6:F15" si="2">C6*0.0933+0.086363636</f>
+        <v>12.028763635999999</v>
+      </c>
+    </row>
+    <row r="7" spans="1:6" x14ac:dyDescent="0.25">
+      <c r="A7">
+        <v>64</v>
+      </c>
+      <c r="B7" s="3">
+        <v>160</v>
+      </c>
+      <c r="C7" s="3">
+        <f t="shared" si="0"/>
+        <v>96</v>
+      </c>
+      <c r="D7" s="5">
+        <v>59.2</v>
+      </c>
+      <c r="E7" s="5">
+        <f t="shared" si="1"/>
+        <v>9.2000000000000028</v>
+      </c>
+      <c r="F7" s="10">
+        <f t="shared" si="2"/>
+        <v>9.0431636359999992</v>
+      </c>
+    </row>
+    <row r="8" spans="1:6" x14ac:dyDescent="0.25">
+      <c r="A8">
+        <v>96</v>
+      </c>
+      <c r="B8" s="3">
+        <v>160</v>
+      </c>
+      <c r="C8" s="3">
+        <f t="shared" si="0"/>
+        <v>64</v>
+      </c>
+      <c r="D8" s="5">
+        <v>56.4</v>
+      </c>
+      <c r="E8" s="5">
+        <f t="shared" si="1"/>
+        <v>6.3999999999999986</v>
+      </c>
+      <c r="F8" s="10">
+        <f t="shared" si="2"/>
+        <v>6.0575636359999994</v>
+      </c>
+    </row>
+    <row r="9" spans="1:6" x14ac:dyDescent="0.25">
+      <c r="A9">
+        <v>128</v>
+      </c>
+      <c r="B9" s="3">
+        <v>160</v>
+      </c>
+      <c r="C9" s="3">
+        <f t="shared" si="0"/>
+        <v>32</v>
+      </c>
+      <c r="D9" s="5">
+        <v>53.35</v>
+      </c>
+      <c r="E9" s="5">
+        <f t="shared" si="1"/>
+        <v>3.3500000000000014</v>
+      </c>
+      <c r="F9" s="10">
+        <f t="shared" si="2"/>
+        <v>3.071963636</v>
+      </c>
+    </row>
+    <row r="10" spans="1:6" x14ac:dyDescent="0.25">
+      <c r="A10">
+        <v>160</v>
+      </c>
+      <c r="B10" s="3">
+        <v>160</v>
+      </c>
+      <c r="C10" s="3">
+        <f t="shared" si="0"/>
+        <v>0</v>
+      </c>
+      <c r="D10" s="5">
+        <v>50</v>
+      </c>
+      <c r="E10" s="5">
+        <f t="shared" si="1"/>
+        <v>0</v>
+      </c>
+      <c r="F10" s="10">
+        <f t="shared" si="2"/>
+        <v>8.6363635999999994E-2</v>
+      </c>
+    </row>
+    <row r="11" spans="1:6" x14ac:dyDescent="0.25">
+      <c r="A11">
+        <v>192</v>
+      </c>
+      <c r="B11" s="3">
+        <v>160</v>
+      </c>
+      <c r="C11" s="3">
+        <f t="shared" si="0"/>
+        <v>-32</v>
+      </c>
+      <c r="D11" s="5">
+        <v>46.9</v>
+      </c>
+      <c r="E11" s="5">
+        <f t="shared" si="1"/>
+        <v>-3.1000000000000014</v>
+      </c>
+      <c r="F11" s="10">
+        <f t="shared" si="2"/>
+        <v>-2.8992363639999996</v>
+      </c>
+    </row>
+    <row r="12" spans="1:6" x14ac:dyDescent="0.25">
+      <c r="A12">
+        <v>224</v>
+      </c>
+      <c r="B12" s="3">
+        <v>160</v>
+      </c>
+      <c r="C12" s="3">
+        <f t="shared" si="0"/>
+        <v>-64</v>
+      </c>
+      <c r="D12" s="5">
+        <v>43.9</v>
+      </c>
+      <c r="E12" s="5">
+        <f t="shared" si="1"/>
+        <v>-6.1000000000000014</v>
+      </c>
+      <c r="F12" s="10">
+        <f t="shared" si="2"/>
+        <v>-5.8848363639999999</v>
+      </c>
+    </row>
+    <row r="13" spans="1:6" x14ac:dyDescent="0.25">
+      <c r="A13">
+        <v>256</v>
+      </c>
+      <c r="B13" s="3">
+        <v>160</v>
+      </c>
+      <c r="C13" s="3">
+        <f t="shared" si="0"/>
+        <v>-96</v>
+      </c>
+      <c r="D13" s="5">
+        <v>40.799999999999997</v>
+      </c>
+      <c r="E13" s="5">
+        <f t="shared" si="1"/>
+        <v>-9.2000000000000028</v>
+      </c>
+      <c r="F13" s="10">
+        <f t="shared" si="2"/>
+        <v>-8.8704363639999997</v>
+      </c>
+    </row>
+    <row r="14" spans="1:6" x14ac:dyDescent="0.25">
+      <c r="A14">
+        <v>288</v>
+      </c>
+      <c r="B14" s="3">
+        <v>160</v>
+      </c>
+      <c r="C14" s="3">
+        <f t="shared" si="0"/>
+        <v>-128</v>
+      </c>
+      <c r="D14" s="5">
+        <v>38.299999999999997</v>
+      </c>
+      <c r="E14" s="5">
+        <f t="shared" si="1"/>
+        <v>-11.700000000000003</v>
+      </c>
+      <c r="F14" s="10">
+        <f t="shared" si="2"/>
+        <v>-11.856036363999999</v>
+      </c>
+    </row>
+    <row r="15" spans="1:6" x14ac:dyDescent="0.25">
+      <c r="A15">
+        <v>315</v>
+      </c>
+      <c r="B15" s="3">
+        <v>160</v>
+      </c>
+      <c r="C15" s="3">
+        <f t="shared" si="0"/>
+        <v>-155</v>
+      </c>
+      <c r="D15" s="5">
+        <v>35.799999999999997</v>
+      </c>
+      <c r="E15" s="5">
+        <f t="shared" si="1"/>
+        <v>-14.200000000000003</v>
+      </c>
+      <c r="F15" s="10">
+        <f t="shared" si="2"/>
+        <v>-14.375136363999999</v>
+      </c>
+    </row>
+    <row r="16" spans="1:6" x14ac:dyDescent="0.25">
+      <c r="C16" s="3"/>
+      <c r="D16" s="5"/>
+      <c r="E16" s="5"/>
+    </row>
+    <row r="17" spans="1:6" ht="18" thickBot="1" x14ac:dyDescent="0.35">
+      <c r="A17" s="1" t="s">
+        <v>3</v>
+      </c>
+      <c r="C17" s="3"/>
+      <c r="D17" s="5"/>
+      <c r="E17" s="5"/>
+    </row>
+    <row r="18" spans="1:6" ht="15.75" thickTop="1" x14ac:dyDescent="0.25">
+      <c r="A18">
+        <v>5</v>
+      </c>
+      <c r="B18" s="3">
+        <v>120</v>
+      </c>
+      <c r="C18" s="3">
+        <f t="shared" si="0"/>
+        <v>115</v>
+      </c>
+      <c r="D18" s="5">
+        <v>59.5</v>
+      </c>
+      <c r="E18" s="5">
+        <f t="shared" si="1"/>
+        <v>9.5</v>
+      </c>
+      <c r="F18" s="10">
+        <f>C18*0.0812+0.2091</f>
+        <v>9.5470999999999986</v>
+      </c>
+    </row>
+    <row r="19" spans="1:6" x14ac:dyDescent="0.25">
+      <c r="A19">
+        <v>24</v>
+      </c>
+      <c r="B19" s="3">
+        <v>120</v>
+      </c>
+      <c r="C19" s="3">
+        <f t="shared" si="0"/>
+        <v>96</v>
+      </c>
+      <c r="D19" s="5">
+        <v>58.3</v>
+      </c>
+      <c r="E19" s="5">
+        <f t="shared" si="1"/>
+        <v>8.2999999999999972</v>
+      </c>
+      <c r="F19" s="10">
+        <f t="shared" ref="F19:F28" si="3">C19*0.0812+0.2091</f>
+        <v>8.0042999999999989</v>
+      </c>
+    </row>
+    <row r="20" spans="1:6" x14ac:dyDescent="0.25">
+      <c r="A20">
+        <v>48</v>
+      </c>
+      <c r="B20" s="3">
+        <v>120</v>
+      </c>
+      <c r="C20" s="3">
+        <f t="shared" si="0"/>
+        <v>72</v>
+      </c>
+      <c r="D20" s="5">
+        <v>56.2</v>
+      </c>
+      <c r="E20" s="5">
+        <f t="shared" si="1"/>
+        <v>6.2000000000000028</v>
+      </c>
+      <c r="F20" s="10">
+        <f t="shared" si="3"/>
+        <v>6.0554999999999994</v>
+      </c>
+    </row>
+    <row r="21" spans="1:6" x14ac:dyDescent="0.25">
+      <c r="A21">
+        <v>72</v>
+      </c>
+      <c r="B21" s="3">
+        <v>120</v>
+      </c>
+      <c r="C21" s="3">
+        <f t="shared" si="0"/>
+        <v>48</v>
+      </c>
+      <c r="D21" s="5">
+        <v>54.4</v>
+      </c>
+      <c r="E21" s="5">
+        <f t="shared" si="1"/>
+        <v>4.3999999999999986</v>
+      </c>
+      <c r="F21" s="10">
+        <f t="shared" si="3"/>
+        <v>4.1067</v>
+      </c>
+    </row>
+    <row r="22" spans="1:6" x14ac:dyDescent="0.25">
+      <c r="A22">
+        <v>96</v>
+      </c>
+      <c r="B22" s="3">
+        <v>120</v>
+      </c>
+      <c r="C22" s="3">
+        <f t="shared" si="0"/>
+        <v>24</v>
+      </c>
+      <c r="D22" s="5">
+        <v>52.1</v>
+      </c>
+      <c r="E22" s="5">
+        <f t="shared" si="1"/>
+        <v>2.1000000000000014</v>
+      </c>
+      <c r="F22" s="10">
+        <f t="shared" si="3"/>
+        <v>2.1578999999999997</v>
+      </c>
+    </row>
+    <row r="23" spans="1:6" x14ac:dyDescent="0.25">
+      <c r="A23">
+        <v>120</v>
+      </c>
+      <c r="B23" s="3">
+        <v>120</v>
+      </c>
+      <c r="C23" s="3">
+        <f t="shared" si="0"/>
+        <v>0</v>
+      </c>
+      <c r="D23" s="5">
+        <v>50</v>
+      </c>
+      <c r="E23" s="5">
+        <f t="shared" si="1"/>
+        <v>0</v>
+      </c>
+      <c r="F23" s="10">
+        <f t="shared" si="3"/>
+        <v>0.20910000000000001</v>
+      </c>
+    </row>
+    <row r="24" spans="1:6" x14ac:dyDescent="0.25">
+      <c r="A24">
+        <v>144</v>
+      </c>
+      <c r="B24" s="3">
+        <v>120</v>
+      </c>
+      <c r="C24" s="3">
+        <f t="shared" si="0"/>
+        <v>-24</v>
+      </c>
+      <c r="D24" s="5">
+        <v>47.9</v>
+      </c>
+      <c r="E24" s="5">
+        <f t="shared" si="1"/>
+        <v>-2.1000000000000014</v>
+      </c>
+      <c r="F24" s="10">
+        <f t="shared" si="3"/>
+        <v>-1.7396999999999998</v>
+      </c>
+    </row>
+    <row r="25" spans="1:6" x14ac:dyDescent="0.25">
+      <c r="A25">
+        <v>168</v>
+      </c>
+      <c r="B25" s="3">
+        <v>120</v>
+      </c>
+      <c r="C25" s="3">
+        <f t="shared" si="0"/>
+        <v>-48</v>
+      </c>
+      <c r="D25" s="5">
+        <v>45.6</v>
+      </c>
+      <c r="E25" s="5">
+        <f t="shared" si="1"/>
+        <v>-4.3999999999999986</v>
+      </c>
+      <c r="F25" s="10">
+        <f t="shared" si="3"/>
+        <v>-3.6884999999999999</v>
+      </c>
+    </row>
+    <row r="26" spans="1:6" x14ac:dyDescent="0.25">
+      <c r="A26">
+        <v>192</v>
+      </c>
+      <c r="B26" s="3">
+        <v>120</v>
+      </c>
+      <c r="C26" s="3">
+        <f t="shared" si="0"/>
+        <v>-72</v>
+      </c>
+      <c r="D26" s="5">
+        <v>43.8</v>
+      </c>
+      <c r="E26" s="5">
+        <f t="shared" si="1"/>
+        <v>-6.2000000000000028</v>
+      </c>
+      <c r="F26" s="10">
+        <f t="shared" si="3"/>
+        <v>-5.6372999999999989</v>
+      </c>
+    </row>
+    <row r="27" spans="1:6" x14ac:dyDescent="0.25">
+      <c r="A27">
+        <v>216</v>
+      </c>
+      <c r="B27" s="3">
+        <v>120</v>
+      </c>
+      <c r="C27" s="3">
+        <f t="shared" si="0"/>
+        <v>-96</v>
+      </c>
+      <c r="D27" s="5">
+        <v>43</v>
+      </c>
+      <c r="E27" s="5">
+        <f t="shared" si="1"/>
+        <v>-7</v>
+      </c>
+      <c r="F27" s="10">
+        <f t="shared" si="3"/>
+        <v>-7.5860999999999992</v>
+      </c>
+    </row>
+    <row r="28" spans="1:6" x14ac:dyDescent="0.25">
+      <c r="A28">
+        <v>235</v>
+      </c>
+      <c r="B28" s="3">
+        <v>120</v>
+      </c>
+      <c r="C28" s="3">
+        <f t="shared" si="0"/>
+        <v>-115</v>
+      </c>
+      <c r="D28" s="5">
+        <v>41.5</v>
+      </c>
+      <c r="E28" s="5">
+        <f t="shared" si="1"/>
+        <v>-8.5</v>
+      </c>
+      <c r="F28" s="10">
+        <f t="shared" si="3"/>
+        <v>-9.1288999999999998</v>
+      </c>
+    </row>
+  </sheetData>
+  <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
+  <pageSetup orientation="portrait" r:id="rId1"/>
+  <drawing r:id="rId2"/>
+</worksheet>
+</file>
+
+<file path=xl/worksheets/sheet2.xml><?xml version="1.0" encoding="utf-8"?>
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
   <dimension ref="A1:I18"/>
   <sheetViews>
     <sheetView workbookViewId="0">
-      <selection activeCell="G7" sqref="G7"/>
+      <selection activeCell="B18" sqref="B18"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -2846,493 +3713,232 @@
 </worksheet>
 </file>
 
-<file path=xl/worksheets/sheet2.xml><?xml version="1.0" encoding="utf-8"?>
+<file path=xl/worksheets/sheet3.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
-  <dimension ref="A1:E28"/>
+  <dimension ref="A1:I18"/>
   <sheetViews>
-    <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="Q24" sqref="Q24"/>
+    <sheetView workbookViewId="0">
+      <selection activeCell="B17" sqref="B17"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
   <cols>
-    <col min="1" max="1" width="15.28515625" customWidth="1"/>
-    <col min="2" max="4" width="13.7109375" customWidth="1"/>
-    <col min="5" max="5" width="15.5703125" customWidth="1"/>
+    <col min="1" max="1" width="27" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:5" s="2" customFormat="1" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
-      <c r="A1" s="2" t="s">
-        <v>5</v>
-      </c>
-    </row>
-    <row r="2" spans="1:5" s="2" customFormat="1" ht="30.75" thickBot="1" x14ac:dyDescent="0.3">
-      <c r="A2" s="2" t="s">
-        <v>0</v>
-      </c>
-      <c r="B2" s="2" t="s">
+    <row r="1" spans="1:9" x14ac:dyDescent="0.25">
+      <c r="A1" t="s">
+        <v>10</v>
+      </c>
+    </row>
+    <row r="2" spans="1:9" ht="15.75" thickBot="1" x14ac:dyDescent="0.3"/>
+    <row r="3" spans="1:9" x14ac:dyDescent="0.25">
+      <c r="A3" s="9" t="s">
+        <v>11</v>
+      </c>
+      <c r="B3" s="9"/>
+    </row>
+    <row r="4" spans="1:9" x14ac:dyDescent="0.25">
+      <c r="A4" s="6" t="s">
+        <v>12</v>
+      </c>
+      <c r="B4" s="6">
+        <v>0.99760386202579909</v>
+      </c>
+    </row>
+    <row r="5" spans="1:9" x14ac:dyDescent="0.25">
+      <c r="A5" s="6" t="s">
+        <v>13</v>
+      </c>
+      <c r="B5" s="6">
+        <v>0.99521346552878953</v>
+      </c>
+    </row>
+    <row r="6" spans="1:9" x14ac:dyDescent="0.25">
+      <c r="A6" s="6" t="s">
+        <v>14</v>
+      </c>
+      <c r="B6" s="6">
+        <v>0.99468162836532181</v>
+      </c>
+    </row>
+    <row r="7" spans="1:9" x14ac:dyDescent="0.25">
+      <c r="A7" s="6" t="s">
+        <v>15</v>
+      </c>
+      <c r="B7" s="6">
+        <v>0.46372107652835542</v>
+      </c>
+    </row>
+    <row r="8" spans="1:9" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
+      <c r="A8" s="7" t="s">
+        <v>16</v>
+      </c>
+      <c r="B8" s="7">
+        <v>11</v>
+      </c>
+    </row>
+    <row r="10" spans="1:9" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
+      <c r="A10" t="s">
+        <v>17</v>
+      </c>
+    </row>
+    <row r="11" spans="1:9" x14ac:dyDescent="0.25">
+      <c r="A11" s="8"/>
+      <c r="B11" s="8" t="s">
+        <v>22</v>
+      </c>
+      <c r="C11" s="8" t="s">
+        <v>23</v>
+      </c>
+      <c r="D11" s="8" t="s">
+        <v>24</v>
+      </c>
+      <c r="E11" s="8" t="s">
+        <v>25</v>
+      </c>
+      <c r="F11" s="8" t="s">
+        <v>26</v>
+      </c>
+    </row>
+    <row r="12" spans="1:9" x14ac:dyDescent="0.25">
+      <c r="A12" s="6" t="s">
+        <v>18</v>
+      </c>
+      <c r="B12" s="6">
         <v>1</v>
       </c>
-      <c r="D2" s="2" t="s">
-        <v>2</v>
-      </c>
-      <c r="E2" s="4" t="s">
-        <v>6</v>
-      </c>
-    </row>
-    <row r="3" spans="1:5" x14ac:dyDescent="0.25">
-      <c r="B3" t="s">
-        <v>4</v>
-      </c>
-    </row>
-    <row r="4" spans="1:5" ht="18" thickBot="1" x14ac:dyDescent="0.35">
-      <c r="A4" s="1" t="s">
-        <v>2</v>
-      </c>
-      <c r="C4" t="s">
-        <v>8</v>
-      </c>
-      <c r="D4" t="s">
-        <v>7</v>
-      </c>
-      <c r="E4" t="s">
+      <c r="C12" s="6">
+        <v>402.39375577774143</v>
+      </c>
+      <c r="D12" s="6">
+        <v>402.39375577774143</v>
+      </c>
+      <c r="E12" s="6">
+        <v>1871.2747695921228</v>
+      </c>
+      <c r="F12" s="6">
+        <v>9.4129783025355299E-12</v>
+      </c>
+    </row>
+    <row r="13" spans="1:9" x14ac:dyDescent="0.25">
+      <c r="A13" s="6" t="s">
+        <v>19</v>
+      </c>
+      <c r="B13" s="6">
         <v>9</v>
       </c>
-    </row>
-    <row r="5" spans="1:5" ht="15.75" thickTop="1" x14ac:dyDescent="0.25">
-      <c r="A5">
-        <v>5</v>
-      </c>
-      <c r="B5" s="3">
-        <v>160</v>
-      </c>
-      <c r="C5" s="3">
-        <f>B5-A5</f>
-        <v>155</v>
-      </c>
-      <c r="D5" s="5">
-        <v>64</v>
-      </c>
-      <c r="E5" s="5">
-        <f>D5-50</f>
-        <v>14</v>
-      </c>
-    </row>
-    <row r="6" spans="1:5" x14ac:dyDescent="0.25">
-      <c r="A6">
-        <v>32</v>
-      </c>
-      <c r="B6" s="3">
-        <v>160</v>
-      </c>
-      <c r="C6" s="3">
-        <f t="shared" ref="C6:C28" si="0">B6-A6</f>
-        <v>128</v>
-      </c>
-      <c r="D6" s="5">
-        <v>62.3</v>
-      </c>
-      <c r="E6" s="5">
-        <f t="shared" ref="E6:E28" si="1">D6-50</f>
-        <v>12.299999999999997</v>
-      </c>
-    </row>
-    <row r="7" spans="1:5" x14ac:dyDescent="0.25">
-      <c r="A7">
-        <v>64</v>
-      </c>
-      <c r="B7" s="3">
-        <v>160</v>
-      </c>
-      <c r="C7" s="3">
-        <f t="shared" si="0"/>
-        <v>96</v>
-      </c>
-      <c r="D7" s="5">
-        <v>59.2</v>
-      </c>
-      <c r="E7" s="5">
-        <f t="shared" si="1"/>
-        <v>9.2000000000000028</v>
-      </c>
-    </row>
-    <row r="8" spans="1:5" x14ac:dyDescent="0.25">
-      <c r="A8">
-        <v>96</v>
-      </c>
-      <c r="B8" s="3">
-        <v>160</v>
-      </c>
-      <c r="C8" s="3">
-        <f t="shared" si="0"/>
-        <v>64</v>
-      </c>
-      <c r="D8" s="5">
-        <v>56.4</v>
-      </c>
-      <c r="E8" s="5">
-        <f t="shared" si="1"/>
-        <v>6.3999999999999986</v>
-      </c>
-    </row>
-    <row r="9" spans="1:5" x14ac:dyDescent="0.25">
-      <c r="A9">
-        <v>128</v>
-      </c>
-      <c r="B9" s="3">
-        <v>160</v>
-      </c>
-      <c r="C9" s="3">
-        <f t="shared" si="0"/>
-        <v>32</v>
-      </c>
-      <c r="D9" s="5">
-        <v>53.35</v>
-      </c>
-      <c r="E9" s="5">
-        <f t="shared" si="1"/>
-        <v>3.3500000000000014</v>
-      </c>
-    </row>
-    <row r="10" spans="1:5" x14ac:dyDescent="0.25">
-      <c r="A10">
-        <v>160</v>
-      </c>
-      <c r="B10" s="3">
-        <v>160</v>
-      </c>
-      <c r="C10" s="3">
-        <f t="shared" si="0"/>
-        <v>0</v>
-      </c>
-      <c r="D10" s="5">
-        <v>50</v>
-      </c>
-      <c r="E10" s="5">
-        <f t="shared" si="1"/>
-        <v>0</v>
-      </c>
-    </row>
-    <row r="11" spans="1:5" x14ac:dyDescent="0.25">
-      <c r="A11">
-        <v>192</v>
-      </c>
-      <c r="B11" s="3">
-        <v>160</v>
-      </c>
-      <c r="C11" s="3">
-        <f t="shared" si="0"/>
-        <v>-32</v>
-      </c>
-      <c r="D11" s="5">
-        <v>46.9</v>
-      </c>
-      <c r="E11" s="5">
-        <f t="shared" si="1"/>
-        <v>-3.1000000000000014</v>
-      </c>
-    </row>
-    <row r="12" spans="1:5" x14ac:dyDescent="0.25">
-      <c r="A12">
-        <v>224</v>
-      </c>
-      <c r="B12" s="3">
-        <v>160</v>
-      </c>
-      <c r="C12" s="3">
-        <f t="shared" si="0"/>
-        <v>-64</v>
-      </c>
-      <c r="D12" s="5">
-        <v>43.9</v>
-      </c>
-      <c r="E12" s="5">
-        <f t="shared" si="1"/>
-        <v>-6.1000000000000014</v>
-      </c>
-    </row>
-    <row r="13" spans="1:5" x14ac:dyDescent="0.25">
-      <c r="A13">
-        <v>256</v>
-      </c>
-      <c r="B13" s="3">
-        <v>160</v>
-      </c>
-      <c r="C13" s="3">
-        <f t="shared" si="0"/>
-        <v>-96</v>
-      </c>
-      <c r="D13" s="5">
-        <v>40.799999999999997</v>
-      </c>
-      <c r="E13" s="5">
-        <f t="shared" si="1"/>
-        <v>-9.2000000000000028</v>
-      </c>
-    </row>
-    <row r="14" spans="1:5" x14ac:dyDescent="0.25">
-      <c r="A14">
-        <v>288</v>
-      </c>
-      <c r="B14" s="3">
-        <v>160</v>
-      </c>
-      <c r="C14" s="3">
-        <f t="shared" si="0"/>
-        <v>-128</v>
-      </c>
-      <c r="D14" s="5">
-        <v>38.299999999999997</v>
-      </c>
-      <c r="E14" s="5">
-        <f t="shared" si="1"/>
-        <v>-11.700000000000003</v>
-      </c>
-    </row>
-    <row r="15" spans="1:5" x14ac:dyDescent="0.25">
-      <c r="A15">
-        <v>315</v>
-      </c>
-      <c r="B15" s="3">
-        <v>160</v>
-      </c>
-      <c r="C15" s="3">
-        <f t="shared" si="0"/>
-        <v>-155</v>
-      </c>
-      <c r="D15" s="5">
-        <v>35.799999999999997</v>
-      </c>
-      <c r="E15" s="5">
-        <f t="shared" si="1"/>
-        <v>-14.200000000000003</v>
-      </c>
-    </row>
-    <row r="16" spans="1:5" x14ac:dyDescent="0.25">
-      <c r="C16" s="3"/>
-      <c r="D16" s="5"/>
-      <c r="E16" s="5"/>
-    </row>
-    <row r="17" spans="1:5" ht="18" thickBot="1" x14ac:dyDescent="0.35">
-      <c r="A17" s="1" t="s">
-        <v>3</v>
-      </c>
-      <c r="C17" s="3"/>
-      <c r="D17" s="5"/>
-      <c r="E17" s="5"/>
-    </row>
-    <row r="18" spans="1:5" ht="15.75" thickTop="1" x14ac:dyDescent="0.25">
-      <c r="A18">
-        <v>5</v>
-      </c>
-      <c r="B18" s="3">
-        <v>120</v>
-      </c>
-      <c r="C18" s="3">
-        <f t="shared" si="0"/>
-        <v>115</v>
-      </c>
-      <c r="D18" s="5">
-        <v>59.5</v>
-      </c>
-      <c r="E18" s="5">
-        <f t="shared" si="1"/>
-        <v>9.5</v>
-      </c>
-    </row>
-    <row r="19" spans="1:5" x14ac:dyDescent="0.25">
-      <c r="A19">
-        <v>24</v>
-      </c>
-      <c r="B19" s="3">
-        <v>120</v>
-      </c>
-      <c r="C19" s="3">
-        <f t="shared" si="0"/>
-        <v>96</v>
-      </c>
-      <c r="D19" s="5">
-        <v>58.3</v>
-      </c>
-      <c r="E19" s="5">
-        <f t="shared" si="1"/>
-        <v>8.2999999999999972</v>
-      </c>
-    </row>
-    <row r="20" spans="1:5" x14ac:dyDescent="0.25">
-      <c r="A20">
-        <v>48</v>
-      </c>
-      <c r="B20" s="3">
-        <v>120</v>
-      </c>
-      <c r="C20" s="3">
-        <f t="shared" si="0"/>
-        <v>72</v>
-      </c>
-      <c r="D20" s="5">
-        <v>56.2</v>
-      </c>
-      <c r="E20" s="5">
-        <f t="shared" si="1"/>
-        <v>6.2000000000000028</v>
-      </c>
-    </row>
-    <row r="21" spans="1:5" x14ac:dyDescent="0.25">
-      <c r="A21">
-        <v>72</v>
-      </c>
-      <c r="B21" s="3">
-        <v>120</v>
-      </c>
-      <c r="C21" s="3">
-        <f t="shared" si="0"/>
-        <v>48</v>
-      </c>
-      <c r="D21" s="5">
-        <v>54.4</v>
-      </c>
-      <c r="E21" s="5">
-        <f t="shared" si="1"/>
-        <v>4.3999999999999986</v>
-      </c>
-    </row>
-    <row r="22" spans="1:5" x14ac:dyDescent="0.25">
-      <c r="A22">
-        <v>96</v>
-      </c>
-      <c r="B22" s="3">
-        <v>120</v>
-      </c>
-      <c r="C22" s="3">
-        <f t="shared" si="0"/>
-        <v>24</v>
-      </c>
-      <c r="D22" s="5">
-        <v>52.1</v>
-      </c>
-      <c r="E22" s="5">
-        <f t="shared" si="1"/>
-        <v>2.1000000000000014</v>
-      </c>
-    </row>
-    <row r="23" spans="1:5" x14ac:dyDescent="0.25">
-      <c r="A23">
-        <v>120</v>
-      </c>
-      <c r="B23" s="3">
-        <v>120</v>
-      </c>
-      <c r="C23" s="3">
-        <f t="shared" si="0"/>
-        <v>0</v>
-      </c>
-      <c r="D23" s="5">
-        <v>50</v>
-      </c>
-      <c r="E23" s="5">
-        <f t="shared" si="1"/>
-        <v>0</v>
-      </c>
-    </row>
-    <row r="24" spans="1:5" x14ac:dyDescent="0.25">
-      <c r="A24">
-        <v>144</v>
-      </c>
-      <c r="B24" s="3">
-        <v>120</v>
-      </c>
-      <c r="C24" s="3">
-        <f t="shared" si="0"/>
-        <v>-24</v>
-      </c>
-      <c r="D24" s="5">
-        <v>47.9</v>
-      </c>
-      <c r="E24" s="5">
-        <f t="shared" si="1"/>
-        <v>-2.1000000000000014</v>
-      </c>
-    </row>
-    <row r="25" spans="1:5" x14ac:dyDescent="0.25">
-      <c r="A25">
-        <v>168</v>
-      </c>
-      <c r="B25" s="3">
-        <v>120</v>
-      </c>
-      <c r="C25" s="3">
-        <f t="shared" si="0"/>
-        <v>-48</v>
-      </c>
-      <c r="D25" s="5">
-        <v>45.6</v>
-      </c>
-      <c r="E25" s="5">
-        <f t="shared" si="1"/>
-        <v>-4.3999999999999986</v>
-      </c>
-    </row>
-    <row r="26" spans="1:5" x14ac:dyDescent="0.25">
-      <c r="A26">
-        <v>192</v>
-      </c>
-      <c r="B26" s="3">
-        <v>120</v>
-      </c>
-      <c r="C26" s="3">
-        <f t="shared" si="0"/>
-        <v>-72</v>
-      </c>
-      <c r="D26" s="5">
-        <v>43.8</v>
-      </c>
-      <c r="E26" s="5">
-        <f t="shared" si="1"/>
-        <v>-6.2000000000000028</v>
-      </c>
-    </row>
-    <row r="27" spans="1:5" x14ac:dyDescent="0.25">
-      <c r="A27">
-        <v>216</v>
-      </c>
-      <c r="B27" s="3">
-        <v>120</v>
-      </c>
-      <c r="C27" s="3">
-        <f t="shared" si="0"/>
-        <v>-96</v>
-      </c>
-      <c r="D27" s="5">
-        <v>43</v>
-      </c>
-      <c r="E27" s="5">
-        <f t="shared" si="1"/>
-        <v>-7</v>
-      </c>
-    </row>
-    <row r="28" spans="1:5" x14ac:dyDescent="0.25">
-      <c r="A28">
-        <v>235</v>
-      </c>
-      <c r="B28" s="3">
-        <v>120</v>
-      </c>
-      <c r="C28" s="3">
-        <f t="shared" si="0"/>
-        <v>-115</v>
-      </c>
-      <c r="D28" s="5">
-        <v>41.5</v>
-      </c>
-      <c r="E28" s="5">
-        <f t="shared" si="1"/>
-        <v>-8.5</v>
+      <c r="C13" s="6">
+        <v>1.9353351313495517</v>
+      </c>
+      <c r="D13" s="6">
+        <v>0.21503723681661685</v>
+      </c>
+      <c r="E13" s="6"/>
+      <c r="F13" s="6"/>
+    </row>
+    <row r="14" spans="1:9" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
+      <c r="A14" s="7" t="s">
+        <v>20</v>
+      </c>
+      <c r="B14" s="7">
+        <v>10</v>
+      </c>
+      <c r="C14" s="7">
+        <v>404.32909090909101</v>
+      </c>
+      <c r="D14" s="7"/>
+      <c r="E14" s="7"/>
+      <c r="F14" s="7"/>
+    </row>
+    <row r="15" spans="1:9" ht="15.75" thickBot="1" x14ac:dyDescent="0.3"/>
+    <row r="16" spans="1:9" x14ac:dyDescent="0.25">
+      <c r="A16" s="8"/>
+      <c r="B16" s="8" t="s">
+        <v>27</v>
+      </c>
+      <c r="C16" s="8" t="s">
+        <v>15</v>
+      </c>
+      <c r="D16" s="8" t="s">
+        <v>28</v>
+      </c>
+      <c r="E16" s="8" t="s">
+        <v>29</v>
+      </c>
+      <c r="F16" s="8" t="s">
+        <v>30</v>
+      </c>
+      <c r="G16" s="8" t="s">
+        <v>31</v>
+      </c>
+      <c r="H16" s="8" t="s">
+        <v>36</v>
+      </c>
+      <c r="I16" s="8" t="s">
+        <v>37</v>
+      </c>
+    </row>
+    <row r="17" spans="1:9" x14ac:dyDescent="0.25">
+      <c r="A17" s="6" t="s">
+        <v>21</v>
+      </c>
+      <c r="B17" s="6">
+        <v>0.20909090909090883</v>
+      </c>
+      <c r="C17" s="6">
+        <v>0.13981716529311247</v>
+      </c>
+      <c r="D17" s="6">
+        <v>1.4954595070824888</v>
+      </c>
+      <c r="E17" s="6">
+        <v>0.16900881510319213</v>
+      </c>
+      <c r="F17" s="6">
+        <v>-0.10719749285904617</v>
+      </c>
+      <c r="G17" s="6">
+        <v>0.52537931104086377</v>
+      </c>
+      <c r="H17" s="6">
+        <v>-0.1853945436366809</v>
+      </c>
+      <c r="I17" s="6">
+        <v>0.60357636181849861</v>
+      </c>
+    </row>
+    <row r="18" spans="1:9" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
+      <c r="A18" s="7" t="s">
+        <v>34</v>
+      </c>
+      <c r="B18" s="7">
+        <v>8.1212915915423664E-2</v>
+      </c>
+      <c r="C18" s="7">
+        <v>1.8773978791229286E-3</v>
+      </c>
+      <c r="D18" s="7">
+        <v>43.258233546830375</v>
+      </c>
+      <c r="E18" s="7">
+        <v>9.4129783025355622E-12</v>
+      </c>
+      <c r="F18" s="7">
+        <v>7.6965946855743567E-2</v>
+      </c>
+      <c r="G18" s="7">
+        <v>8.5459884975103761E-2</v>
+      </c>
+      <c r="H18" s="7">
+        <v>7.5915954338903219E-2</v>
+      </c>
+      <c r="I18" s="7">
+        <v>8.6509877491944109E-2</v>
       </c>
     </row>
   </sheetData>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
   <pageSetup orientation="portrait" r:id="rId1"/>
-  <drawing r:id="rId2"/>
 </worksheet>
 </file>
</xml_diff>